<commit_message>
Start more entry on airlines
</commit_message>
<xml_diff>
--- a/$INDIGO.xlsx
+++ b/$INDIGO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E979F9-C11F-4EEB-9F00-74D8687E0078}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C944AA-8ACB-434A-86AC-724F66846A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{65B6E1EB-2A96-42C5-A051-A9BED254A02E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15360" xr2:uid="{65B6E1EB-2A96-42C5-A051-A9BED254A02E}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>$INDIGO</t>
   </si>
@@ -88,6 +98,9 @@
   </si>
   <si>
     <t>INR</t>
+  </si>
+  <si>
+    <t>Gurgaon, India</t>
   </si>
 </sst>
 </file>
@@ -95,7 +108,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -244,10 +257,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -257,32 +296,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,211 +619,221 @@
   <dimension ref="B2:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C26" sqref="C26:D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+    <row r="2" spans="2:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B5" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="6" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="27"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="4">
         <v>1779.1</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="6" t="s">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="17">
         <v>385.26</v>
       </c>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="6" t="s">
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="17">
         <f>C6*C7</f>
         <v>685416.06599999999</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="5"/>
       <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
+      <c r="C9" s="17"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="6" t="s">
+      <c r="C10" s="17"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="17">
         <f>C9-C10</f>
         <v>0</v>
       </c>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="9" t="s">
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="25">
+      <c r="C12" s="18">
         <f>C8-C11</f>
         <v>685416.06599999999</v>
       </c>
-      <c r="D12" s="10"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+      <c r="D12" s="7"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B15" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="19"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="22"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="3" t="s">
+      <c r="C15" s="26"/>
+      <c r="D15" s="27"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B20" s="13"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B23" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="11" t="s">
+      <c r="C23" s="26"/>
+      <c r="D23" s="27"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B24" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="13"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="11" t="s">
+      <c r="C24" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="29"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B25" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="13"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="11"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="13"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="13"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="11"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="13"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="11" t="s">
+      <c r="C25" s="28">
+        <v>2005</v>
+      </c>
+      <c r="D25" s="29"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B26" s="8"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B27" s="8"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="22"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B28" s="8"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="22"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B29" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="27"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="14" t="s">
+      <c r="C29" s="19"/>
+      <c r="D29" s="20"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B30" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="16"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="3" t="s">
+      <c r="C30" s="23"/>
+      <c r="D30" s="24"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B33" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="11" t="s">
+      <c r="C33" s="26"/>
+      <c r="D33" s="27"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B34" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="13"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="11" t="s">
+      <c r="C34" s="21"/>
+      <c r="D34" s="22"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B35" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="13"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="14" t="s">
+      <c r="C35" s="21"/>
+      <c r="D35" s="22"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B36" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="16"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C27:D27"/>
@@ -812,12 +841,6 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="C34:D34"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>